<commit_message>
configuracion correcta de feature excel y cambios menores
</commit_message>
<xml_diff>
--- a/testData/data.xlsx
+++ b/testData/data.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benja\OneDrive\Desktop\AutomatizacionEVA2\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DCB23DC-761E-4F4C-85C9-C65F64C3B523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBEB9E93-EECC-4FC5-8910-4C0C74B25E17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3500" yWindow="2690" windowWidth="22100" windowHeight="11170" xr2:uid="{4DC31BE8-C152-4FC9-A9A7-B32F959A6A82}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>User</t>
   </si>
@@ -86,13 +86,20 @@
     <t>800003 Checking</t>
   </si>
   <si>
-    <t>Transfer Complete</t>
+    <t>Prueba NO OK</t>
+  </si>
+  <si>
+    <t>Prueba OK</t>
+  </si>
+  <si>
+    <t>successfully transferred</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -501,7 +508,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -565,9 +572,11 @@
         <v>10</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
@@ -588,7 +597,9 @@
       <c r="F4" s="2">
         <v>1000000</v>
       </c>
-      <c r="G4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
@@ -607,9 +618,11 @@
         <v>100</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="1"/>

</xml_diff>